<commit_message>
updated weekly pump data
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/weekly_Pump_Data.xlsx
+++ b/heliostrome/jip_project/results/weekly_Pump_Data.xlsx
@@ -461,10 +461,10 @@
         <v>38389</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>74.19408395296784</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>235.6160305053561</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>38396</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>89.43834202308427</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>322.8997759563496</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         <v>38403</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>81.40379101139183</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>295.5660860094558</v>
       </c>
     </row>
     <row r="5">
@@ -494,10 +494,10 @@
         <v>38410</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>86.83916451945294</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>321.1505416764683</v>
       </c>
     </row>
     <row r="6">
@@ -505,10 +505,10 @@
         <v>38417</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>12.89914685508182</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>48.79759880703651</v>
       </c>
     </row>
     <row r="7">
@@ -549,10 +549,10 @@
         <v>38445</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>33.88210938269473</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>144.5162077920627</v>
       </c>
     </row>
     <row r="11">
@@ -560,10 +560,10 @@
         <v>38452</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>70.47520533542121</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>273.6202019474335</v>
       </c>
     </row>
     <row r="12">
@@ -571,10 +571,10 @@
         <v>38459</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>76.36126498340384</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>326.9761422393509</v>
       </c>
     </row>
     <row r="13">
@@ -582,10 +582,10 @@
         <v>38466</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>67.29923937340671</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>320.7905813088454</v>
       </c>
     </row>
     <row r="14">
@@ -593,10 +593,10 @@
         <v>38473</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>68.12926509896874</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>284.4968567438901</v>
       </c>
     </row>
     <row r="15">
@@ -604,10 +604,10 @@
         <v>38480</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>76.68185093707488</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>295.1250822512637</v>
       </c>
     </row>
     <row r="16">
@@ -615,10 +615,10 @@
         <v>38487</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>71.72916689551374</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>307.6276947554144</v>
       </c>
     </row>
     <row r="17">
@@ -626,10 +626,10 @@
         <v>38494</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>49.52876982530729</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>207.7216895924848</v>
       </c>
     </row>
     <row r="18">
@@ -637,10 +637,10 @@
         <v>38501</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>62.3870836582288</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>282.1812468481443</v>
       </c>
     </row>
     <row r="19">
@@ -648,10 +648,10 @@
         <v>38508</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>17.3163181737962</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>85.2829193704211</v>
       </c>
     </row>
     <row r="20">
@@ -4091,10 +4091,10 @@
         <v>40699</v>
       </c>
       <c r="B332" t="n">
-        <v>0</v>
+        <v>49.53641628222108</v>
       </c>
       <c r="C332" t="n">
-        <v>0</v>
+        <v>195.6177744368306</v>
       </c>
     </row>
     <row r="333">
@@ -4102,10 +4102,10 @@
         <v>40706</v>
       </c>
       <c r="B333" t="n">
-        <v>0</v>
+        <v>67.65603271884665</v>
       </c>
       <c r="C333" t="n">
-        <v>0</v>
+        <v>265.4257390016767</v>
       </c>
     </row>
     <row r="334">
@@ -4113,10 +4113,10 @@
         <v>40713</v>
       </c>
       <c r="B334" t="n">
-        <v>0</v>
+        <v>53.43321041568568</v>
       </c>
       <c r="C334" t="n">
-        <v>0</v>
+        <v>180.5277599601374</v>
       </c>
     </row>
     <row r="335">
@@ -4124,10 +4124,10 @@
         <v>40720</v>
       </c>
       <c r="B335" t="n">
-        <v>0</v>
+        <v>51.88458076800471</v>
       </c>
       <c r="C335" t="n">
-        <v>0</v>
+        <v>185.3590561792269</v>
       </c>
     </row>
     <row r="336">
@@ -4135,10 +4135,10 @@
         <v>40727</v>
       </c>
       <c r="B336" t="n">
-        <v>0</v>
+        <v>22.99160156496697</v>
       </c>
       <c r="C336" t="n">
-        <v>0</v>
+        <v>82.42496309863617</v>
       </c>
     </row>
     <row r="337">
@@ -4146,10 +4146,10 @@
         <v>40734</v>
       </c>
       <c r="B337" t="n">
-        <v>0</v>
+        <v>90.35570131241732</v>
       </c>
       <c r="C337" t="n">
-        <v>0</v>
+        <v>312.9842346499702</v>
       </c>
     </row>
     <row r="338">
@@ -4157,10 +4157,10 @@
         <v>40741</v>
       </c>
       <c r="B338" t="n">
-        <v>0</v>
+        <v>66.47221519592834</v>
       </c>
       <c r="C338" t="n">
-        <v>0</v>
+        <v>236.0801356833313</v>
       </c>
     </row>
     <row r="339">
@@ -4168,10 +4168,10 @@
         <v>40748</v>
       </c>
       <c r="B339" t="n">
-        <v>0</v>
+        <v>63.49660768735646</v>
       </c>
       <c r="C339" t="n">
-        <v>0</v>
+        <v>227.3674781209431</v>
       </c>
     </row>
     <row r="340">
@@ -4179,10 +4179,10 @@
         <v>40755</v>
       </c>
       <c r="B340" t="n">
-        <v>0</v>
+        <v>71.00953652726186</v>
       </c>
       <c r="C340" t="n">
-        <v>0</v>
+        <v>292.6441106717706</v>
       </c>
     </row>
     <row r="341">
@@ -4762,10 +4762,10 @@
         <v>41126</v>
       </c>
       <c r="B393" t="n">
-        <v>0</v>
+        <v>52.3238815982878</v>
       </c>
       <c r="C393" t="n">
-        <v>0</v>
+        <v>184.4766616097709</v>
       </c>
     </row>
     <row r="394">
@@ -4773,10 +4773,10 @@
         <v>41133</v>
       </c>
       <c r="B394" t="n">
-        <v>0</v>
+        <v>81.74441741544337</v>
       </c>
       <c r="C394" t="n">
-        <v>0</v>
+        <v>284.273573943435</v>
       </c>
     </row>
     <row r="395">
@@ -4784,10 +4784,10 @@
         <v>41140</v>
       </c>
       <c r="B395" t="n">
-        <v>0</v>
+        <v>66.50176335058171</v>
       </c>
       <c r="C395" t="n">
-        <v>0</v>
+        <v>255.997714289286</v>
       </c>
     </row>
     <row r="396">
@@ -4795,10 +4795,10 @@
         <v>41147</v>
       </c>
       <c r="B396" t="n">
-        <v>0</v>
+        <v>54.39357174783888</v>
       </c>
       <c r="C396" t="n">
-        <v>0</v>
+        <v>208.9845211338032</v>
       </c>
     </row>
     <row r="397">
@@ -4806,10 +4806,10 @@
         <v>41154</v>
       </c>
       <c r="B397" t="n">
-        <v>0</v>
+        <v>55.33902895397608</v>
       </c>
       <c r="C397" t="n">
-        <v>0</v>
+        <v>211.6259761430322</v>
       </c>
     </row>
     <row r="398">
@@ -5004,10 +5004,10 @@
         <v>41280</v>
       </c>
       <c r="B415" t="n">
-        <v>0</v>
+        <v>89.72959203905191</v>
       </c>
       <c r="C415" t="n">
-        <v>0</v>
+        <v>270.8278930788219</v>
       </c>
     </row>
     <row r="416">
@@ -5015,10 +5015,10 @@
         <v>41287</v>
       </c>
       <c r="B416" t="n">
-        <v>0</v>
+        <v>89.95104541581306</v>
       </c>
       <c r="C416" t="n">
-        <v>0</v>
+        <v>251.9425414092616</v>
       </c>
     </row>
     <row r="417">
@@ -5026,10 +5026,10 @@
         <v>41294</v>
       </c>
       <c r="B417" t="n">
-        <v>0</v>
+        <v>95.8267613971673</v>
       </c>
       <c r="C417" t="n">
-        <v>0</v>
+        <v>319.263771972892</v>
       </c>
     </row>
     <row r="418">
@@ -5037,10 +5037,10 @@
         <v>41301</v>
       </c>
       <c r="B418" t="n">
-        <v>0</v>
+        <v>112.96153866474</v>
       </c>
       <c r="C418" t="n">
-        <v>0</v>
+        <v>341.0152590276041</v>
       </c>
     </row>
     <row r="419">
@@ -5048,10 +5048,10 @@
         <v>41308</v>
       </c>
       <c r="B419" t="n">
-        <v>0</v>
+        <v>57.09796487215972</v>
       </c>
       <c r="C419" t="n">
-        <v>0</v>
+        <v>186.1405822876012</v>
       </c>
     </row>
     <row r="420">
@@ -5433,10 +5433,10 @@
         <v>41553</v>
       </c>
       <c r="B454" t="n">
-        <v>0</v>
+        <v>41.09573104696092</v>
       </c>
       <c r="C454" t="n">
-        <v>0</v>
+        <v>159.770758626355</v>
       </c>
     </row>
     <row r="455">
@@ -5444,10 +5444,10 @@
         <v>41560</v>
       </c>
       <c r="B455" t="n">
-        <v>0</v>
+        <v>80.68603951886227</v>
       </c>
       <c r="C455" t="n">
-        <v>0</v>
+        <v>310.0930647615996</v>
       </c>
     </row>
     <row r="456">
@@ -5455,10 +5455,10 @@
         <v>41567</v>
       </c>
       <c r="B456" t="n">
-        <v>0</v>
+        <v>73.16593037566265</v>
       </c>
       <c r="C456" t="n">
-        <v>0</v>
+        <v>288.1524420535704</v>
       </c>
     </row>
     <row r="457">
@@ -5466,10 +5466,10 @@
         <v>41574</v>
       </c>
       <c r="B457" t="n">
-        <v>0</v>
+        <v>40.61371398592992</v>
       </c>
       <c r="C457" t="n">
-        <v>0</v>
+        <v>152.3069586493511</v>
       </c>
     </row>
     <row r="458">
@@ -5477,10 +5477,10 @@
         <v>41581</v>
       </c>
       <c r="B458" t="n">
-        <v>0</v>
+        <v>43.84693099188979</v>
       </c>
       <c r="C458" t="n">
-        <v>0</v>
+        <v>171.1594880868015</v>
       </c>
     </row>
     <row r="459">
@@ -6049,10 +6049,10 @@
         <v>41945</v>
       </c>
       <c r="B510" t="n">
-        <v>0</v>
+        <v>23.46702885390863</v>
       </c>
       <c r="C510" t="n">
-        <v>0</v>
+        <v>94.03088363335192</v>
       </c>
     </row>
     <row r="511">
@@ -6060,10 +6060,10 @@
         <v>41952</v>
       </c>
       <c r="B511" t="n">
-        <v>0</v>
+        <v>71.49740029740083</v>
       </c>
       <c r="C511" t="n">
-        <v>0</v>
+        <v>301.6934536168001</v>
       </c>
     </row>
     <row r="512">
@@ -6071,10 +6071,10 @@
         <v>41959</v>
       </c>
       <c r="B512" t="n">
-        <v>0</v>
+        <v>81.13655678641017</v>
       </c>
       <c r="C512" t="n">
-        <v>0</v>
+        <v>307.490211741934</v>
       </c>
     </row>
     <row r="513">
@@ -6082,10 +6082,10 @@
         <v>41966</v>
       </c>
       <c r="B513" t="n">
-        <v>0</v>
+        <v>86.95960832714304</v>
       </c>
       <c r="C513" t="n">
-        <v>0</v>
+        <v>309.3345309898328</v>
       </c>
     </row>
     <row r="514">
@@ -6093,10 +6093,10 @@
         <v>41973</v>
       </c>
       <c r="B514" t="n">
-        <v>0</v>
+        <v>87.81513156460471</v>
       </c>
       <c r="C514" t="n">
-        <v>0</v>
+        <v>299.7865204695406</v>
       </c>
     </row>
     <row r="515">
@@ -6104,10 +6104,10 @@
         <v>41980</v>
       </c>
       <c r="B515" t="n">
-        <v>0</v>
+        <v>90.34599235316769</v>
       </c>
       <c r="C515" t="n">
-        <v>0</v>
+        <v>314.4756660099475</v>
       </c>
     </row>
     <row r="516">
@@ -6115,10 +6115,10 @@
         <v>41987</v>
       </c>
       <c r="B516" t="n">
-        <v>0</v>
+        <v>47.05255936190578</v>
       </c>
       <c r="C516" t="n">
-        <v>0</v>
+        <v>149.3019578533691</v>
       </c>
     </row>
     <row r="517">
@@ -6126,10 +6126,10 @@
         <v>41994</v>
       </c>
       <c r="B517" t="n">
-        <v>0</v>
+        <v>77.77085003318966</v>
       </c>
       <c r="C517" t="n">
-        <v>0</v>
+        <v>251.7955005061134</v>
       </c>
     </row>
     <row r="518">
@@ -6137,10 +6137,10 @@
         <v>42001</v>
       </c>
       <c r="B518" t="n">
-        <v>0</v>
+        <v>72.25796910256551</v>
       </c>
       <c r="C518" t="n">
-        <v>0</v>
+        <v>232.5003231081802</v>
       </c>
     </row>
     <row r="519">
@@ -6148,10 +6148,10 @@
         <v>42008</v>
       </c>
       <c r="B519" t="n">
-        <v>0</v>
+        <v>19.28184452671116</v>
       </c>
       <c r="C519" t="n">
-        <v>0</v>
+        <v>62.06945016401679</v>
       </c>
     </row>
     <row r="520">
@@ -6819,10 +6819,10 @@
         <v>42435</v>
       </c>
       <c r="B580" t="n">
-        <v>0</v>
+        <v>65.22965875316933</v>
       </c>
       <c r="C580" t="n">
-        <v>0</v>
+        <v>264.1628533872337</v>
       </c>
     </row>
     <row r="581">
@@ -6830,10 +6830,10 @@
         <v>42442</v>
       </c>
       <c r="B581" t="n">
-        <v>0</v>
+        <v>78.63398330660458</v>
       </c>
       <c r="C581" t="n">
-        <v>0</v>
+        <v>311.2252101021177</v>
       </c>
     </row>
     <row r="582">
@@ -6841,10 +6841,10 @@
         <v>42449</v>
       </c>
       <c r="B582" t="n">
-        <v>0</v>
+        <v>66.90199116984282</v>
       </c>
       <c r="C582" t="n">
-        <v>0</v>
+        <v>272.1300033031059</v>
       </c>
     </row>
     <row r="583">
@@ -6852,10 +6852,10 @@
         <v>42456</v>
       </c>
       <c r="B583" t="n">
-        <v>0</v>
+        <v>71.65319751390444</v>
       </c>
       <c r="C583" t="n">
-        <v>0</v>
+        <v>313.1579700885604</v>
       </c>
     </row>
     <row r="584">
@@ -6863,10 +6863,10 @@
         <v>42463</v>
       </c>
       <c r="B584" t="n">
-        <v>0</v>
+        <v>43.94523252154485</v>
       </c>
       <c r="C584" t="n">
-        <v>0</v>
+        <v>159.7777856250967</v>
       </c>
     </row>
     <row r="585">
@@ -7105,10 +7105,10 @@
         <v>42617</v>
       </c>
       <c r="B606" t="n">
-        <v>0</v>
+        <v>35.94738360435686</v>
       </c>
       <c r="C606" t="n">
-        <v>0</v>
+        <v>131.2784698312382</v>
       </c>
     </row>
     <row r="607">
@@ -7116,10 +7116,10 @@
         <v>42624</v>
       </c>
       <c r="B607" t="n">
-        <v>0</v>
+        <v>68.58709693293379</v>
       </c>
       <c r="C607" t="n">
-        <v>0</v>
+        <v>259.9260202829755</v>
       </c>
     </row>
     <row r="608">
@@ -7127,10 +7127,10 @@
         <v>42631</v>
       </c>
       <c r="B608" t="n">
-        <v>0</v>
+        <v>58.7103703390521</v>
       </c>
       <c r="C608" t="n">
-        <v>0</v>
+        <v>243.0631912795414</v>
       </c>
     </row>
     <row r="609">
@@ -7138,10 +7138,10 @@
         <v>42638</v>
       </c>
       <c r="B609" t="n">
-        <v>0</v>
+        <v>49.90356429910386</v>
       </c>
       <c r="C609" t="n">
-        <v>0</v>
+        <v>195.2176278500575</v>
       </c>
     </row>
     <row r="610">
@@ -7149,10 +7149,10 @@
         <v>42645</v>
       </c>
       <c r="B610" t="n">
-        <v>0</v>
+        <v>43.8055337938171</v>
       </c>
       <c r="C610" t="n">
-        <v>0</v>
+        <v>177.4631878721851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>